<commit_message>
Calculated the predicted DM/cm of twigs and branches. file Branch_15N ready to calculate recovered 15N
</commit_message>
<xml_diff>
--- a/15N_experiment/15N_branches/weights_per_length.xlsx
+++ b/15N_experiment/15N_branches/weights_per_length.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s1373890\Daniele_Repo\15N_experiment\15N_branches\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$D$23</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -110,7 +110,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -155,7 +155,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -436,7 +436,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,6 +467,12 @@
         <f>8.5+5.4+7.1+9+5.2+7.9+5.5+5.7+7.7+7.4</f>
         <v>69.400000000000006</v>
       </c>
+      <c r="C2">
+        <v>4.4550000000000001</v>
+      </c>
+      <c r="D2">
+        <v>1.028</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -476,6 +482,12 @@
         <f>15.2+4.1+6.7+16+12.3+7.1+13.5+7.9+11.6+7.2</f>
         <v>101.60000000000001</v>
       </c>
+      <c r="C3">
+        <v>7.5030000000000001</v>
+      </c>
+      <c r="D3">
+        <v>2.4849999999999999</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -485,6 +497,12 @@
         <f>11+7.6+7.7+8.9+9.3+10+9.2+9.9+9.7+11.1</f>
         <v>94.4</v>
       </c>
+      <c r="C4">
+        <v>7.4580000000000002</v>
+      </c>
+      <c r="D4">
+        <v>2.29</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -494,6 +512,12 @@
         <f>12.3+17.6+9.4+6.6+9+15.1+14.1+10.4+6.5+7.9</f>
         <v>108.9</v>
       </c>
+      <c r="C5">
+        <v>8.9870000000000001</v>
+      </c>
+      <c r="D5">
+        <v>3.1680000000000001</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -503,6 +527,12 @@
         <f>15.6+11.3+12.7+5.6+4.9+10.8+9.9+14.5+9+12.6</f>
         <v>106.89999999999999</v>
       </c>
+      <c r="C6">
+        <v>7.9329999999999998</v>
+      </c>
+      <c r="D6">
+        <v>2.544</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -512,6 +542,12 @@
         <f>11+13+12+14+21+10+9.5+10.5</f>
         <v>101</v>
       </c>
+      <c r="C7">
+        <v>11.677</v>
+      </c>
+      <c r="D7">
+        <v>8.7279999999999998</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -521,6 +557,12 @@
         <f>19+16+21+13+15+8</f>
         <v>92</v>
       </c>
+      <c r="C8">
+        <v>10.223000000000001</v>
+      </c>
+      <c r="D8">
+        <v>4.96</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -530,6 +572,12 @@
         <f>21+13+11.5+16+11+15+13+15</f>
         <v>115.5</v>
       </c>
+      <c r="C9">
+        <v>11.34</v>
+      </c>
+      <c r="D9">
+        <v>4.8869999999999996</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -539,6 +587,12 @@
         <f>13+18+11+17+13+8+8+8</f>
         <v>96</v>
       </c>
+      <c r="C10">
+        <v>11.093999999999999</v>
+      </c>
+      <c r="D10">
+        <v>4.6139999999999999</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -548,6 +602,12 @@
         <f>7.5+9+9.5+9+8+6.5+6.5+7</f>
         <v>63</v>
       </c>
+      <c r="C11">
+        <v>5.2640000000000002</v>
+      </c>
+      <c r="D11">
+        <v>1.1519999999999999</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -557,6 +617,12 @@
         <f>7.7+7.4+8+7.5+5.6+6+8</f>
         <v>50.2</v>
       </c>
+      <c r="C12">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="D12">
+        <v>0.81100000000000005</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -566,6 +632,12 @@
         <f>8.2+7.7+6.1+8.6+5.5+7.6+6+7.4+4.9+4+5.9+6.3+6.8+4.5</f>
         <v>89.5</v>
       </c>
+      <c r="C13">
+        <v>5.2149999999999999</v>
+      </c>
+      <c r="D13">
+        <v>0.92</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -575,6 +647,12 @@
         <f>7.5+8.5+8+8.7+8.1+7.6+9.5+6.9+10.8+3.4</f>
         <v>79.000000000000014</v>
       </c>
+      <c r="C14">
+        <v>3.2050000000000001</v>
+      </c>
+      <c r="D14">
+        <v>1.1240000000000001</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -584,6 +662,12 @@
         <f>11.2+7.6+4.6+5.5+5.7+3.7+7.5+3.4+5.5+6.4</f>
         <v>61.1</v>
       </c>
+      <c r="C15">
+        <v>2.1219999999999999</v>
+      </c>
+      <c r="D15">
+        <v>0.92400000000000004</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -593,8 +677,14 @@
         <f>7+5.5+12.5+8+7.5+8+9+9.5+5.5+6</f>
         <v>78.5</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>3.2040000000000002</v>
+      </c>
+      <c r="D16">
+        <v>1.282</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -602,8 +692,14 @@
         <f>6.5+6.6+6.5+7+6+5.7+5.9+9.3+9+5.8</f>
         <v>68.3</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>2.4369999999999998</v>
+      </c>
+      <c r="D17">
+        <v>0.77500000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -611,8 +707,14 @@
         <f>13.7+13.6+4.5+7.4+5.9+19+7+9.8+6.1+4.8</f>
         <v>91.799999999999983</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>8.1210000000000004</v>
+      </c>
+      <c r="D18">
+        <v>2.395</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -620,8 +722,14 @@
         <f>17.3+10.9+16.9+15.2+10.1+10.9+7.8+6+8.2+16.1+7.3+7.4+5.3+9.2</f>
         <v>148.6</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>12.663</v>
+      </c>
+      <c r="D19">
+        <v>3.7650000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -629,8 +737,14 @@
         <f>28.6+14.7+5.4+5.4+17.7+21.2+27+36.2+13.7</f>
         <v>169.89999999999998</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>11.397</v>
+      </c>
+      <c r="D20">
+        <v>12.006</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -638,8 +752,14 @@
         <f>9+9+19.5+19+10+10+17+18</f>
         <v>111.5</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>6.125</v>
+      </c>
+      <c r="D21">
+        <v>2.6480000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -647,14 +767,26 @@
         <f>21.8+7.7+7.7+14.2+12.2+11.3+11.2+14.8+16.8+15.1</f>
         <v>132.80000000000001</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>8.8190000000000008</v>
+      </c>
+      <c r="D22">
+        <v>3.7330000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>25</v>
       </c>
       <c r="B23">
         <f>15.5+13.5+14+8.5+7.5+6.5+6.5+8.5</f>
         <v>80.5</v>
+      </c>
+      <c r="C23">
+        <v>3.8519999999999999</v>
+      </c>
+      <c r="D23">
+        <v>1.4470000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>